<commit_message>
Update the xls rubric with the auto grading
</commit_message>
<xml_diff>
--- a/rubric/Rubric_Geomatics.xlsx
+++ b/rubric/Rubric_Geomatics.xlsx
@@ -1,17 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hugo/www/geo2020/rubric/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E65AD469-0948-6F42-9BDD-BFAB8FD7D2EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="30680" windowHeight="18080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="77">
   <si>
     <t>Research</t>
   </si>
@@ -239,30 +258,27 @@
   </si>
   <si>
     <t xml:space="preserve">Just sufficient level of self-reflection, but should be more open to advise and feedback </t>
+  </si>
+  <si>
+    <t>grade</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
-    <numFmt numFmtId="0" formatCode="General"/>
-    <numFmt numFmtId="59" formatCode="0.0%"/>
-    <numFmt numFmtId="60" formatCode="#,##0%"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.0%"/>
+    <numFmt numFmtId="165" formatCode="#,##0%"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="14"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b val="1"/>
+      <b/>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
@@ -272,8 +288,22 @@
       <color indexed="8"/>
       <name val="Tahoma Bold"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -304,8 +334,26 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -348,21 +396,6 @@
         <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
-      </right>
-      <top style="thin">
-        <color indexed="9"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="9"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
         <color indexed="10"/>
       </right>
       <top style="thin">
@@ -388,75 +421,175 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color theme="3"/>
+      </right>
+      <top style="thin">
+        <color indexed="9"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color theme="3"/>
+      </right>
+      <top style="thin">
+        <color indexed="9"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="9"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color theme="3"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="3"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="3"/>
+      </left>
+      <right style="thin">
+        <color theme="3"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="3"/>
+      </left>
+      <right style="thin">
+        <color theme="3"/>
+      </right>
+      <top style="thin">
+        <color theme="3"/>
+      </top>
+      <bottom style="thin">
+        <color theme="3"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
+  </cellStyleXfs>
+  <cellXfs count="34">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-  </cellStyleXfs>
-  <cellXfs count="21">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="59" fontId="2" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="2" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="9" fontId="1" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="5" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="59" fontId="2" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="59" fontId="2" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
+    <xf numFmtId="9" fontId="1" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="2" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="60" fontId="2" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="2" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -466,49 +599,113 @@
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ff84b4df"/>
-      <rgbColor rgb="ffa7a7a7"/>
-      <rgbColor rgb="ffadcdea"/>
-      <rgbColor rgb="ffe4e4e4"/>
-      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FF84B4DF"/>
+      <rgbColor rgb="FFA7A7A7"/>
+      <rgbColor rgb="FFADCDEA"/>
+      <rgbColor rgb="FFE4E4E4"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>983781</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>82766</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>969671</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>642977</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>25399</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>151830</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>732366</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>246375</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
+    <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="Shape 2"/>
+        <xdr:cNvPr id="2" name="Shape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11994681" y="10168471"/>
-          <a:ext cx="794219" cy="259565"/>
+          <a:off x="969671" y="10040977"/>
+          <a:ext cx="792806" cy="266620"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -521,7 +718,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{C572A759-6A51-4108-AA02-DFA0A04FC94B}">
-            <ma14:wrappingTextBoxFlag xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" val="1"/>
+            <ma14:wrappingTextBoxFlag xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" val="1"/>
           </a:ext>
         </a:extLst>
       </xdr:spPr>
@@ -546,7 +743,7 @@
             <a:buFontTx/>
             <a:buNone/>
             <a:tabLst/>
-            <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none">
+            <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" baseline="0">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -558,7 +755,7 @@
             </a:defRPr>
           </a:pPr>
           <a:r>
-            <a:rPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none">
+            <a:rPr sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" baseline="0">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -579,7 +776,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office Theme">
       <a:dk1>
@@ -781,7 +978,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -800,7 +997,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -830,7 +1027,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -856,7 +1053,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -882,7 +1079,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -908,7 +1105,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -934,7 +1131,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -960,7 +1157,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -986,7 +1183,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1012,7 +1209,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1038,7 +1235,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1051,9 +1248,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -1070,7 +1273,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1089,7 +1292,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1115,7 +1318,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1141,7 +1344,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1167,7 +1370,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1193,7 +1396,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1219,7 +1422,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1245,7 +1448,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1271,7 +1474,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1297,7 +1500,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1323,7 +1526,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1336,9 +1539,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1352,7 +1561,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1371,7 +1580,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1401,7 +1610,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1427,7 +1636,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1453,7 +1662,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1479,7 +1688,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1505,7 +1714,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1531,7 +1740,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1557,7 +1766,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1583,7 +1792,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1609,7 +1818,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1622,37 +1831,49 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="B2:H18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B1:I19"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="13.5" style="1" customWidth="1"/>
     <col min="2" max="2" width="35" style="1" customWidth="1"/>
-    <col min="3" max="3" width="5.35156" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8.1640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="24" style="1" customWidth="1"/>
-    <col min="5" max="5" width="22.1719" style="1" customWidth="1"/>
+    <col min="5" max="5" width="22.1640625" style="1" customWidth="1"/>
     <col min="6" max="6" width="23" style="1" customWidth="1"/>
     <col min="7" max="7" width="21.5" style="1" customWidth="1"/>
     <col min="8" max="8" width="23" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.85156" style="1" customWidth="1"/>
+    <col min="9" max="9" width="15.6640625" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="35" customHeight="1"/>
-    <row r="2" ht="13.55" customHeight="1">
+    <row r="1" spans="2:9" ht="35" customHeight="1">
+      <c r="I1" s="20"/>
+    </row>
+    <row r="2" spans="2:9" ht="13.5" customHeight="1">
       <c r="B2" s="2"/>
       <c r="C2" s="3"/>
       <c r="D2" s="4">
@@ -1667,341 +1888,390 @@
       <c r="G2" s="4">
         <v>7</v>
       </c>
-      <c r="H2" s="5">
+      <c r="H2" s="21">
         <v>6</v>
       </c>
+      <c r="I2" s="25" t="s">
+        <v>76</v>
+      </c>
     </row>
-    <row r="3" ht="13.55" customHeight="1">
-      <c r="B3" t="s" s="6">
+    <row r="3" spans="2:9" ht="13.5" customHeight="1">
+      <c r="B3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="6">
         <v>0.5</v>
       </c>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="26"/>
     </row>
-    <row r="4" ht="42" customHeight="1">
-      <c r="B4" t="s" s="9">
+    <row r="4" spans="2:9" ht="42" customHeight="1">
+      <c r="B4" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C4" s="9">
         <v>0.05</v>
       </c>
-      <c r="D4" t="s" s="11">
+      <c r="D4" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E4" t="s" s="11">
+      <c r="E4" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="F4" t="s" s="11">
+      <c r="F4" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="G4" t="s" s="11">
+      <c r="G4" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="H4" t="s" s="11">
+      <c r="H4" s="23" t="s">
         <v>6</v>
       </c>
+      <c r="I4" s="27">
+        <v>6</v>
+      </c>
     </row>
-    <row r="5" ht="84.75" customHeight="1">
-      <c r="B5" t="s" s="12">
+    <row r="5" spans="2:9" ht="84.75" customHeight="1">
+      <c r="B5" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="13">
+      <c r="C5" s="9">
         <v>0.1</v>
       </c>
-      <c r="D5" t="s" s="11">
+      <c r="D5" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E5" t="s" s="11">
+      <c r="E5" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="F5" t="s" s="11">
+      <c r="F5" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="G5" t="s" s="11">
+      <c r="G5" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="H5" t="s" s="11">
+      <c r="H5" s="23" t="s">
         <v>12</v>
       </c>
+      <c r="I5" s="27">
+        <v>6</v>
+      </c>
     </row>
-    <row r="6" ht="53.25" customHeight="1">
-      <c r="B6" t="s" s="12">
+    <row r="6" spans="2:9" ht="53.25" customHeight="1">
+      <c r="B6" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="9">
         <v>0.15</v>
       </c>
-      <c r="D6" t="s" s="11">
+      <c r="D6" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E6" t="s" s="11">
+      <c r="E6" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F6" t="s" s="11">
+      <c r="F6" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="G6" t="s" s="11">
+      <c r="G6" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="H6" t="s" s="11">
+      <c r="H6" s="23" t="s">
         <v>18</v>
       </c>
+      <c r="I6" s="27">
+        <v>6</v>
+      </c>
     </row>
-    <row r="7" ht="84.75" customHeight="1">
-      <c r="B7" t="s" s="12">
+    <row r="7" spans="2:9" ht="84.75" customHeight="1">
+      <c r="B7" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="10">
+      <c r="C7" s="9">
         <v>0.15</v>
       </c>
-      <c r="D7" t="s" s="11">
+      <c r="D7" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="E7" t="s" s="11">
+      <c r="E7" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="F7" t="s" s="11">
+      <c r="F7" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="G7" t="s" s="11">
+      <c r="G7" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="H7" t="s" s="11">
+      <c r="H7" s="23" t="s">
         <v>24</v>
       </c>
+      <c r="I7" s="27">
+        <v>6</v>
+      </c>
     </row>
-    <row r="8" ht="42" customHeight="1">
-      <c r="B8" t="s" s="12">
+    <row r="8" spans="2:9" ht="42" customHeight="1">
+      <c r="B8" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="10">
+      <c r="C8" s="9">
         <v>0.05</v>
       </c>
-      <c r="D8" t="s" s="11">
+      <c r="D8" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="E8" t="s" s="11">
+      <c r="E8" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="F8" t="s" s="11">
+      <c r="F8" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="G8" t="s" s="11">
+      <c r="G8" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="H8" t="s" s="11">
+      <c r="H8" s="23" t="s">
         <v>30</v>
       </c>
+      <c r="I8" s="28">
+        <v>6</v>
+      </c>
     </row>
-    <row r="9" ht="15.75" customHeight="1">
-      <c r="B9" t="s" s="14">
+    <row r="9" spans="2:9" ht="15.75" customHeight="1">
+      <c r="B9" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="15">
+      <c r="C9" s="13">
         <v>0.2</v>
       </c>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="29"/>
     </row>
-    <row r="10" ht="63.75" customHeight="1">
-      <c r="B10" t="s" s="12">
+    <row r="10" spans="2:9" ht="63.75" customHeight="1">
+      <c r="B10" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="10">
+      <c r="C10" s="9">
         <v>0.05</v>
       </c>
-      <c r="D10" t="s" s="11">
+      <c r="D10" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="E10" t="s" s="11">
+      <c r="E10" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="F10" t="s" s="11">
+      <c r="F10" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="G10" t="s" s="11">
+      <c r="G10" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="H10" t="s" s="11">
+      <c r="H10" s="23" t="s">
         <v>37</v>
       </c>
+      <c r="I10" s="27">
+        <v>6</v>
+      </c>
     </row>
-    <row r="11" ht="53.25" customHeight="1">
-      <c r="B11" t="s" s="12">
+    <row r="11" spans="2:9" ht="53.25" customHeight="1">
+      <c r="B11" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="C11" s="13">
+      <c r="C11" s="9">
         <v>0.1</v>
       </c>
-      <c r="D11" t="s" s="11">
+      <c r="D11" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E11" t="s" s="11">
+      <c r="E11" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="F11" t="s" s="11">
+      <c r="F11" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="G11" t="s" s="11">
+      <c r="G11" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="H11" t="s" s="11">
+      <c r="H11" s="23" t="s">
         <v>43</v>
       </c>
+      <c r="I11" s="27">
+        <v>6</v>
+      </c>
     </row>
-    <row r="12" ht="31.5" customHeight="1">
-      <c r="B12" t="s" s="12">
+    <row r="12" spans="2:9" ht="31.5" customHeight="1">
+      <c r="B12" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="C12" s="10">
+      <c r="C12" s="9">
         <v>0.05</v>
       </c>
-      <c r="D12" t="s" s="11">
+      <c r="D12" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="E12" t="s" s="11">
+      <c r="E12" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="F12" t="s" s="11">
+      <c r="F12" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="G12" t="s" s="11">
+      <c r="G12" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="H12" t="s" s="11">
+      <c r="H12" s="23" t="s">
         <v>49</v>
       </c>
+      <c r="I12" s="27">
+        <v>6</v>
+      </c>
     </row>
-    <row r="13" ht="13.55" customHeight="1">
-      <c r="B13" t="s" s="14">
+    <row r="13" spans="2:9" ht="13.5" customHeight="1">
+      <c r="B13" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="C13" s="17">
+      <c r="C13" s="15">
         <v>0.15</v>
       </c>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="16"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="24"/>
+      <c r="I13" s="30"/>
     </row>
-    <row r="14" ht="52.5" customHeight="1">
-      <c r="B14" t="s" s="12">
+    <row r="14" spans="2:9" ht="52.5" customHeight="1">
+      <c r="B14" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="C14" s="18">
-        <v>0.075</v>
-      </c>
-      <c r="D14" t="s" s="11">
+      <c r="C14" s="16">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="D14" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="E14" t="s" s="11">
+      <c r="E14" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="F14" t="s" s="11">
+      <c r="F14" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="G14" t="s" s="11">
+      <c r="G14" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="H14" t="s" s="11">
+      <c r="H14" s="23" t="s">
         <v>56</v>
       </c>
+      <c r="I14" s="27">
+        <v>6</v>
+      </c>
     </row>
-    <row r="15" ht="63" customHeight="1">
-      <c r="B15" t="s" s="19">
+    <row r="15" spans="2:9" ht="63" customHeight="1">
+      <c r="B15" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="C15" s="20">
-        <v>0.07000000000000001</v>
-      </c>
-      <c r="D15" t="s" s="11">
+      <c r="C15" s="18">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="D15" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="E15" t="s" s="11">
+      <c r="E15" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="F15" t="s" s="11">
+      <c r="F15" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="G15" t="s" s="11">
+      <c r="G15" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="H15" t="s" s="11">
+      <c r="H15" s="23" t="s">
         <v>62</v>
       </c>
+      <c r="I15" s="27">
+        <v>6</v>
+      </c>
     </row>
-    <row r="16" ht="15.75" customHeight="1">
-      <c r="B16" t="s" s="14">
+    <row r="16" spans="2:9" ht="15.75" customHeight="1">
+      <c r="B16" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="C16" s="17">
+      <c r="C16" s="15">
         <v>0.15</v>
       </c>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="16"/>
-      <c r="H16" s="16"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="19"/>
+      <c r="I16" s="31"/>
     </row>
-    <row r="17" ht="63.75" customHeight="1">
-      <c r="B17" t="s" s="12">
+    <row r="17" spans="2:9" ht="63.75" customHeight="1">
+      <c r="B17" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="C17" s="10">
+      <c r="C17" s="9">
         <v>0.08</v>
       </c>
-      <c r="D17" t="s" s="11">
+      <c r="D17" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="E17" t="s" s="11">
+      <c r="E17" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="F17" t="s" s="11">
+      <c r="F17" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="G17" t="s" s="11">
+      <c r="G17" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="H17" t="s" s="11">
+      <c r="H17" s="23" t="s">
         <v>69</v>
       </c>
+      <c r="I17" s="32">
+        <v>6</v>
+      </c>
     </row>
-    <row r="18" ht="52.5" customHeight="1">
-      <c r="B18" t="s" s="12">
+    <row r="18" spans="2:9" ht="52.5" customHeight="1">
+      <c r="B18" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="C18" s="10">
-        <v>0.07000000000000001</v>
-      </c>
-      <c r="D18" t="s" s="11">
+      <c r="C18" s="9">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="D18" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="E18" t="s" s="11">
+      <c r="E18" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="F18" t="s" s="11">
+      <c r="F18" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="G18" t="s" s="11">
+      <c r="G18" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="H18" t="s" s="11">
+      <c r="H18" s="23" t="s">
         <v>75</v>
+      </c>
+      <c r="I18" s="32">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" ht="35" customHeight="1">
+      <c r="I19" s="33">
+        <f>I4*0.05+I5*0.1+I6*0.15+I7*0.15+I8*0.05+I10*0.05+I11*0.1+I12*0.05+I14*0.08+I15*0.07+I17*0.08+I18*0.07</f>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.787402" right="0" top="0" bottom="0" header="0.10315" footer="0.10315"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="65" useFirstPageNumber="0" orientation="landscape" pageOrder="downThenOver"/>
+  <pageMargins left="0.78740200000000005" right="0" top="0" bottom="0" header="0.10315000000000001" footer="0.10315000000000001"/>
+  <pageSetup scale="65" orientation="landscape"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>